<commit_message>
Check cities and tables to show
</commit_message>
<xml_diff>
--- a/Team102.2.DataExtractionCode.v1.1/DataSprint.xlsx
+++ b/Team102.2.DataExtractionCode.v1.1/DataSprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iliasasskali/Desktop/Project Management/PMTeam102-2/Team102.2.DataExtractionCode.v1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC716F54-CB09-444C-94F4-0B314095B403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945BDFB5-AD6E-164C-B79A-EE840ABB6F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Poblacio" sheetId="1" r:id="rId1"/>
@@ -191,12 +191,6 @@
     <t>Població total (2020)</t>
   </si>
   <si>
-    <t>Població </t>
-  </si>
-  <si>
-    <t>Densitat de població </t>
-  </si>
-  <si>
     <t>Índex de recanvi poblacional</t>
   </si>
   <si>
@@ -285,6 +279,12 @@
   </si>
   <si>
     <t>Habitatges familiars principals - Per règim de tinença - De propietat (2011)</t>
+  </si>
+  <si>
+    <t>Població</t>
+  </si>
+  <si>
+    <t>Densitat de població</t>
   </si>
 </sst>
 </file>
@@ -694,7 +694,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1391,8 +1391,8 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>31</v>
@@ -1417,7 +1417,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6689,7 +6689,7 @@
   </sheetPr>
   <dimension ref="A1:AF45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -6737,94 +6737,94 @@
         <v>50</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>51</v>
       </c>
       <c r="G1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="Z1" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AE1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE1" s="15" t="s">
-        <v>83</v>
-      </c>
       <c r="AF1" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="15" x14ac:dyDescent="0.2">

</xml_diff>